<commit_message>
fix  speech recognition crs review points
</commit_message>
<xml_diff>
--- a/input documents/CRS/Review/PO_SAG_CRS_ML_SpeechRecog_Review.xlsx
+++ b/input documents/CRS/Review/PO_SAG_CRS_ML_SpeechRecog_Review.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Graduation Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Graduation Project\github_repos\ML_SWProcess_Documents\input documents\CRS\Review\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06A11B9E-24ED-487C-BF8E-FCAB7509CB8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C2A58D4-BC7A-492B-91F8-E3BF3918A322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="60">
   <si>
     <t>DocType_REV_ID</t>
   </si>
@@ -184,6 +184,36 @@
   </si>
   <si>
     <t xml:space="preserve">remove it </t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>CRS_REVIEW_0011</t>
+  </si>
+  <si>
+    <t>the format of the sections titles and content</t>
+  </si>
+  <si>
+    <t>each section title and content</t>
+  </si>
+  <si>
+    <t>edit them to be the same format</t>
+  </si>
+  <si>
+    <t>CRS_REVIEW_0012</t>
+  </si>
+  <si>
+    <t>edit the definition</t>
+  </si>
+  <si>
+    <t>the definition shall be more descreptive</t>
+  </si>
+  <si>
+    <t>43//project descreption//definition</t>
+  </si>
+  <si>
+    <t>V1.2</t>
   </si>
 </sst>
 </file>
@@ -193,7 +223,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -228,20 +258,12 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -252,12 +274,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF3C78D8"/>
         <bgColor rgb="FF3C78D8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF57BB8A"/>
-        <bgColor rgb="FF57BB8A"/>
       </patternFill>
     </fill>
   </fills>
@@ -301,7 +317,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -321,16 +337,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -346,7 +353,30 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF57BB8A"/>
+          <bgColor rgb="FF57BB8A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -630,10 +660,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H103"/>
+  <dimension ref="A1:H104"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -697,7 +727,7 @@
         <v>19</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="67.900000000000006" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -723,7 +753,7 @@
         <v>22</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -749,7 +779,7 @@
         <v>28</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -801,7 +831,7 @@
         <v>24</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -827,128 +857,169 @@
         <v>35</v>
       </c>
       <c r="H7" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="3">
+        <v>44881</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="9">
+        <v>44881</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="9">
+        <v>44881</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="9">
+        <v>44881</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" s="3">
+        <v>44883</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="H12" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="9">
-        <v>44881</v>
-      </c>
-      <c r="C8" s="8" t="s">
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="3">
+        <v>44883</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="H8" s="10" t="s">
+      <c r="D13" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="H13" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" s="12">
-        <v>44881</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="H9" s="13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" s="12">
-        <v>44881</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="H10" s="13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11" s="12">
-        <v>44881</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="H11" s="13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="13"/>
-    </row>
-    <row r="13" spans="1:8" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="6"/>
-    </row>
-    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:8" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="6"/>
+    </row>
     <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1037,40 +1108,51 @@
     <row r="101" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="102" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="103" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="104" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="A2:H7 A11:H11">
-    <cfRule type="expression" dxfId="5" priority="9">
+  <conditionalFormatting sqref="A11:H11 A2:H8">
+    <cfRule type="expression" dxfId="7" priority="13">
       <formula>$H2 = "Closed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:H7 A11:H11">
-    <cfRule type="expression" dxfId="4" priority="10">
+  <conditionalFormatting sqref="A11:H11 A2:H8">
+    <cfRule type="expression" dxfId="6" priority="14">
       <formula>$H2= "Open"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A9:H10">
+    <cfRule type="expression" dxfId="5" priority="7">
+      <formula>$H9 = "Closed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9:H10">
+    <cfRule type="expression" dxfId="4" priority="8">
+      <formula>$H9= "Open"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A13:H13">
+    <cfRule type="expression" dxfId="3" priority="3">
+      <formula>$H13 = "Closed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A13:H13">
+    <cfRule type="expression" dxfId="2" priority="4">
+      <formula>$H13= "Open"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A12:H12">
-    <cfRule type="expression" dxfId="3" priority="7">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>$H12 = "Closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12:H12">
-    <cfRule type="expression" dxfId="2" priority="8">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>$H12= "Open"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A9:H10">
-    <cfRule type="expression" dxfId="1" priority="3">
-      <formula>$H9 = "Closed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A9:H10">
-    <cfRule type="expression" dxfId="0" priority="4">
-      <formula>$H9= "Open"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Open" sqref="H2:H7 H9:H12" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Open" sqref="H2:H13" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Open,Closed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
final approval of crs Speech recognition
</commit_message>
<xml_diff>
--- a/input documents/CRS/Review/PO_SAG_CRS_ML_SpeechRecog_Review.xlsx
+++ b/input documents/CRS/Review/PO_SAG_CRS_ML_SpeechRecog_Review.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Graduation Project\github_repos\ML_SWProcess_Documents\input documents\CRS\Review\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C2A58D4-BC7A-492B-91F8-E3BF3918A322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EEA0EF7-36EA-444D-AEC6-A25A60A9D69E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="59">
   <si>
     <t>DocType_REV_ID</t>
   </si>
@@ -57,9 +57,6 @@
   </si>
   <si>
     <t>Status</t>
-  </si>
-  <si>
-    <t>Open</t>
   </si>
   <si>
     <t>CRS_REVIEW_001</t>
@@ -662,8 +659,8 @@
   </sheetPr>
   <dimension ref="A1:H104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="F3" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -706,314 +703,314 @@
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="3">
         <v>44881</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="67.900000000000006" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="3">
         <v>44881</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="3">
         <v>44881</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="7" t="s">
-        <v>30</v>
-      </c>
       <c r="G4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="3">
         <v>44881</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G5" s="7" t="s">
-        <v>32</v>
-      </c>
       <c r="H5" s="4" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="3">
         <v>44881</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="H6" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="3">
         <v>44881</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="G7" s="7" t="s">
-        <v>35</v>
-      </c>
       <c r="H7" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="3">
         <v>44881</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F8" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="7" t="s">
-        <v>38</v>
-      </c>
       <c r="H8" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B9" s="9">
         <v>44881</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E9" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="G9" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="G9" s="8" t="s">
-        <v>41</v>
-      </c>
       <c r="H9" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B10" s="9">
         <v>44881</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G10" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" s="10" t="s">
         <v>49</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B11" s="9">
         <v>44881</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E11" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="G11" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="G11" s="8" t="s">
-        <v>48</v>
-      </c>
       <c r="H11" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B12" s="3">
         <v>44883</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E12" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="F12" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>54</v>
-      </c>
       <c r="H12" s="4" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B13" s="3">
         <v>44883</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>

</xml_diff>